<commit_message>
added some code and fixed some things
</commit_message>
<xml_diff>
--- a/experimentalData/stdDevForStrainGauge.xlsx
+++ b/experimentalData/stdDevForStrainGauge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\College stuff\UF Stuff\Research\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\College stuff\UF Stuff\Research\Code\experimentalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66256346-AD50-4BA3-8945-BA16D5338E7F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1419631-3607-48A5-AFFF-9074E58E74DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5A386880-2578-490E-A2F7-0C61C8C46988}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5A386880-2578-490E-A2F7-0C61C8C46988}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Column1</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Std. Dev</t>
+  </si>
+  <si>
+    <t>atm pressure</t>
+  </si>
+  <si>
+    <t>Max Deviation</t>
   </si>
 </sst>
 </file>
@@ -1641,12 +1650,12 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1979,19 +1988,19 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1999,7 +2008,7 @@
         <v>1.3023364485981291E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>7.7206735402871897E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2015,7 +2024,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2031,7 +2040,7 @@
         <v>1.1294371687684896E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2039,7 +2048,7 @@
         <v>1.2756283181957818E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2047,7 +2056,7 @@
         <v>-0.80597588631522488</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2055,7 +2064,7 @@
         <v>0.63993445622684753</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2063,7 +2072,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2071,7 +2080,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2079,7 +2088,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2087,7 +2096,7 @@
         <v>2.7869999999999964</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2102,15 +2111,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7061DAE-305B-4AE3-809A-BBDE73F6F235}">
-  <dimension ref="D3:U216"/>
+  <dimension ref="D2:U216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1.4E-2</v>
       </c>
@@ -2123,22 +2148,22 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="4" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="5" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="7" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>1.2999999999999999E-2</v>
       </c>
@@ -2149,7 +2174,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="8" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>1.2E-2</v>
       </c>
@@ -2160,7 +2185,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>1.0999999999999999E-2</v>
       </c>
@@ -2171,7 +2196,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="10" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>0.01</v>
       </c>
@@ -2182,7 +2207,7 @@
         <v>1.006</v>
       </c>
     </row>
-    <row r="11" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -2193,7 +2218,7 @@
         <v>1.252</v>
       </c>
     </row>
-    <row r="12" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -2204,1022 +2229,1022 @@
         <v>1.5509999999999999</v>
       </c>
     </row>
-    <row r="13" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="16" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54">
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>0.01</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61">
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62">
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88">
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94">
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95">
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D103">
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D106">
         <v>0.03</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D109">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110">
         <v>0.03</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114">
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116">
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D117">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122">
         <v>0.02</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D125">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D126">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D127">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D128">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D134">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D135">
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D138">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D139">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D140">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D141">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D142">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D143">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D144">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D145">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D146">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D149">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D150">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D151">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D152">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D153">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D154">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D155">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D156">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D157">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D158">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D159">
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D160">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D161">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D162">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D163">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D164">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D165">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D166">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D167">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D168">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D169">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D170">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D171">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D172">
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D173">
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D174">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D175">
         <v>-4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D176">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D177">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D178">
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D179">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D180">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D181">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D182">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D183">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D184">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D185">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D186">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D187">
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D188">
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D189">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D190">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D191">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D192">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D193">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D194">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D195">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D196">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D197">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D198">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D199">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D200">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D201">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D202">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D203">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D204">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D205">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D206">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D207">
         <v>0.02</v>
       </c>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D208">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D209">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D210">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D211">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D212">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D213">
         <v>0.03</v>
       </c>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D214">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D215">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D216">
         <v>3.1E-2</v>
       </c>

</xml_diff>